<commit_message>
move cursor to top left for Index sheet
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_pooling_v4_12_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_pooling_v4_12_0.xlsx
@@ -2509,7 +2509,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.38"/>
@@ -3878,7 +3878,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="27.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.67"/>
@@ -25964,7 +25964,7 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.2"/>
@@ -26062,7 +26062,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="55.67"/>
   </cols>
@@ -27440,10 +27440,10 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.4375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.78"/>

</xml_diff>